<commit_message>
changed squares; +Volyn region
</commit_message>
<xml_diff>
--- a/private/crops.xlsx
+++ b/private/crops.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="crops" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">Врожайність</t>
   </si>
@@ -100,10 +100,13 @@
     <t xml:space="preserve">ЧЕРНІГІВСЬКА</t>
   </si>
   <si>
-    <t xml:space="preserve">square:null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">square:ChIJiy6tDP5UzUARsED2iIQGAQE</t>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJiy6tDP5UzUARsED2iIQGAQE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJBYI5hgM0JEcRQED2iIQGAQE</t>
   </si>
   <si>
     <t xml:space="preserve">Пшениця озима</t>
@@ -250,6 +253,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -267,12 +271,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -282,6 +280,12 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="204"/>
     </font>
     <font>
@@ -338,7 +342,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,11 +352,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,11 +380,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,7 +396,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Обычный_ЗБОРНИК2005" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -404,17 +408,17 @@
   </sheetPr>
   <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.46428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.53571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,12 +501,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>40.2</v>
@@ -602,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>25.8</v>
@@ -626,7 +633,7 @@
         <v>22.5</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>0.6</v>
@@ -691,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>30.9</v>
@@ -780,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>38.1</v>
@@ -869,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>25.8</v>
@@ -958,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>29.7</v>
@@ -1047,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>25.1</v>
@@ -1136,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>61.6</v>
@@ -1225,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>12.2</v>
@@ -1314,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>50</v>
@@ -1403,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>18</v>
@@ -1492,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>23.4</v>
@@ -1581,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>15.1</v>
@@ -1670,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -1784,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>176.4</v>
@@ -1873,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>263.5</v>
@@ -1962,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>145.2</v>
@@ -2051,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>250.1</v>
@@ -2140,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>218.9</v>
@@ -2229,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>203.3</v>
@@ -2318,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>188.5</v>
@@ -2407,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>87.4</v>
@@ -2496,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>47.8</v>
@@ -2585,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>115.5</v>
@@ -2674,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>115.5</v>
@@ -2763,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>101.5</v>
@@ -2852,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>94.4</v>
@@ -2941,7 +2948,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>71.3</v>
@@ -3030,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -3144,7 +3151,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>476.5</v>
@@ -3233,7 +3240,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>19.4</v>
@@ -3322,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>21.6</v>
@@ -3411,7 +3418,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>25.7</v>
@@ -3500,7 +3507,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>18</v>
@@ -3589,7 +3596,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>12.3</v>
@@ -3678,7 +3685,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>8.3</v>
@@ -3767,7 +3774,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -3881,7 +3888,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -3964,7 +3971,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>14349.5</v>
@@ -4044,7 +4051,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>1834.1</v>
@@ -4124,7 +4131,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>8656.06</v>

</xml_diff>